<commit_message>
oda agadi ko block ko kaam, chyane paakha majhgaun, gravel ghattekulo chanaute
</commit_message>
<xml_diff>
--- a/ofc/estimates/कुर्थली च्यानेपाखा माझगाउँ जोड्ने सडक/V_कुर्थली च्यानेपाखा माझगाउँ जोड्ने सडक.xlsx
+++ b/ofc/estimates/कुर्थली च्यानेपाखा माझगाउँ जोड्ने सडक/V_कुर्थली च्यानेपाखा माझगाउँ जोड्ने सडक.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\कुर्थली च्यानेपाखा माझगाउँ जोड्ने सडक\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\081-082\ofc\ofc\estimates\कुर्थली च्यानेपाखा माझगाउँ जोड्ने सडक\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="200k" sheetId="20" r:id="rId1"/>
@@ -41,12 +41,12 @@
     <definedName name="description_781">[5]Abstract!$B$299</definedName>
     <definedName name="description_783">[1]Abstract!$B$301</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'200k'!$A$1:$K$42</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">V!$A$1:$K$53</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">V!$A$1:$K$54</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'200k'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">V!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">WCR!$1:$12</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="60">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -241,15 +241,18 @@
   </si>
   <si>
     <t>Date:2082/03/02</t>
+  </si>
+  <si>
+    <t>-for road</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -408,7 +411,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -418,7 +421,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -438,14 +441,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -454,7 +457,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -479,7 +482,7 @@
     <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -509,7 +512,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -518,7 +521,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -533,7 +536,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -549,64 +552,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -618,8 +570,59 @@
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1243,130 +1246,130 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.88671875" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="69" t="s">
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="69" t="s">
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-    </row>
-    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="82" t="s">
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+    </row>
+    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="82"/>
-      <c r="K5" s="82"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="73" t="s">
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="79" t="s">
+      <c r="H6" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="84" t="s">
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="85" t="s">
+      <c r="H7" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="68"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1404,7 +1407,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="63">
         <v>1</v>
       </c>
@@ -1427,7 +1430,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="37" t="s">
         <v>51</v>
@@ -1463,7 +1466,7 @@
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="37" t="s">
         <v>42</v>
@@ -1495,7 +1498,7 @@
       <c r="R11" s="25"/>
       <c r="S11" s="25"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="37" t="s">
         <v>40</v>
@@ -1520,7 +1523,7 @@
       <c r="R12" s="25"/>
       <c r="S12" s="25"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="37"/>
       <c r="C13" s="19"/>
@@ -1540,7 +1543,7 @@
       <c r="R13" s="25"/>
       <c r="S13" s="25"/>
     </row>
-    <row r="14" spans="1:19" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <v>2</v>
       </c>
@@ -1564,7 +1567,7 @@
       <c r="R14" s="25"/>
       <c r="S14" s="25"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="37" t="s">
         <v>44</v>
@@ -1600,7 +1603,7 @@
       <c r="R15" s="25"/>
       <c r="S15" s="25"/>
     </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="37" t="s">
         <v>42</v>
@@ -1632,7 +1635,7 @@
       <c r="R16" s="25"/>
       <c r="S16" s="25"/>
     </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="37"/>
       <c r="C17" s="19"/>
@@ -1652,7 +1655,7 @@
       <c r="R17" s="25"/>
       <c r="S17" s="25"/>
     </row>
-    <row r="18" spans="1:19" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>3</v>
       </c>
@@ -1676,7 +1679,7 @@
       <c r="R18" s="25"/>
       <c r="S18" s="25"/>
     </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="37" t="str">
         <f>B15</f>
@@ -1712,7 +1715,7 @@
       <c r="R19" s="25"/>
       <c r="S19" s="25"/>
     </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
       <c r="B20" s="37" t="s">
         <v>42</v>
@@ -1737,7 +1740,7 @@
       </c>
       <c r="K20" s="36"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="37" t="s">
         <v>40</v>
@@ -1755,7 +1758,7 @@
       </c>
       <c r="K21" s="36"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="40"/>
       <c r="B22" s="37"/>
       <c r="C22" s="42"/>
@@ -1768,7 +1771,7 @@
       <c r="J22" s="45"/>
       <c r="K22" s="36"/>
     </row>
-    <row r="23" spans="1:19" ht="69" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
         <v>4</v>
       </c>
@@ -1792,7 +1795,7 @@
       <c r="R23" s="25"/>
       <c r="S23" s="25"/>
     </row>
-    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="37" t="str">
         <f>B10</f>
@@ -1828,7 +1831,7 @@
       <c r="R24" s="25"/>
       <c r="S24" s="25"/>
     </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
       <c r="B25" s="37" t="s">
         <v>42</v>
@@ -1853,7 +1856,7 @@
       </c>
       <c r="K25" s="36"/>
     </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="40"/>
       <c r="B26" s="37" t="s">
         <v>40</v>
@@ -1871,7 +1874,7 @@
       </c>
       <c r="K26" s="36"/>
     </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="40"/>
       <c r="B27" s="37"/>
       <c r="C27" s="42"/>
@@ -1884,7 +1887,7 @@
       <c r="J27" s="45"/>
       <c r="K27" s="36"/>
     </row>
-    <row r="28" spans="1:19" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="135" x14ac:dyDescent="0.25">
       <c r="A28" s="18">
         <v>5</v>
       </c>
@@ -1908,7 +1911,7 @@
       <c r="R28" s="25"/>
       <c r="S28" s="25"/>
     </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="37" t="s">
         <v>51</v>
@@ -1942,7 +1945,7 @@
       <c r="R29" s="25"/>
       <c r="S29" s="25"/>
     </row>
-    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="40"/>
       <c r="B30" s="37" t="s">
         <v>42</v>
@@ -1967,7 +1970,7 @@
       </c>
       <c r="K30" s="36"/>
     </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="40"/>
       <c r="B31" s="37" t="s">
         <v>40</v>
@@ -1985,7 +1988,7 @@
       </c>
       <c r="K31" s="36"/>
     </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="40"/>
       <c r="B32" s="37"/>
       <c r="C32" s="42"/>
@@ -1998,7 +2001,7 @@
       <c r="J32" s="45"/>
       <c r="K32" s="36"/>
     </row>
-    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18">
         <v>6</v>
       </c>
@@ -2028,7 +2031,7 @@
       <c r="K33" s="21"/>
       <c r="M33" s="25"/>
     </row>
-    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
       <c r="B34" s="24"/>
       <c r="C34" s="19"/>
@@ -2048,7 +2051,7 @@
       <c r="R34" s="25"/>
       <c r="S34" s="25"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="40"/>
       <c r="B35" s="46" t="s">
         <v>17</v>
@@ -2066,7 +2069,7 @@
       </c>
       <c r="K35" s="36"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="58"/>
       <c r="B36" s="61"/>
       <c r="C36" s="62"/>
@@ -2079,16 +2082,16 @@
       <c r="J36" s="60"/>
       <c r="K36" s="57"/>
     </row>
-    <row r="37" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="50"/>
       <c r="B37" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="83">
+      <c r="C37" s="66">
         <f>J35</f>
         <v>309587.38791333331</v>
       </c>
-      <c r="D37" s="83"/>
+      <c r="D37" s="66"/>
       <c r="E37" s="39">
         <v>100</v>
       </c>
@@ -2099,15 +2102,15 @@
       <c r="J37" s="54"/>
       <c r="K37" s="55"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="56"/>
       <c r="B38" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="86">
+      <c r="C38" s="69">
         <v>250000</v>
       </c>
-      <c r="D38" s="86"/>
+      <c r="D38" s="69"/>
       <c r="E38" s="39"/>
       <c r="F38" s="49"/>
       <c r="G38" s="48"/>
@@ -2116,16 +2119,16 @@
       <c r="J38" s="48"/>
       <c r="K38" s="49"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="56"/>
       <c r="B39" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="86">
+      <c r="C39" s="69">
         <f>C38-C41-C42</f>
         <v>237500</v>
       </c>
-      <c r="D39" s="86"/>
+      <c r="D39" s="69"/>
       <c r="E39" s="39">
         <f>C39/C37*100</f>
         <v>76.715011422392436</v>
@@ -2137,16 +2140,16 @@
       <c r="J39" s="48"/>
       <c r="K39" s="49"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="56"/>
       <c r="B40" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="83">
+      <c r="C40" s="66">
         <f>C37-C39</f>
         <v>72087.38791333331</v>
       </c>
-      <c r="D40" s="83"/>
+      <c r="D40" s="66"/>
       <c r="E40" s="39">
         <f>100-E39</f>
         <v>23.284988577607564</v>
@@ -2158,16 +2161,16 @@
       <c r="J40" s="48"/>
       <c r="K40" s="49"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="56"/>
       <c r="B41" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="83">
+      <c r="C41" s="66">
         <f>C38*0.03</f>
         <v>7500</v>
       </c>
-      <c r="D41" s="83"/>
+      <c r="D41" s="66"/>
       <c r="E41" s="39">
         <v>3</v>
       </c>
@@ -2178,16 +2181,16 @@
       <c r="J41" s="48"/>
       <c r="K41" s="49"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="56"/>
       <c r="B42" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="83">
+      <c r="C42" s="66">
         <f>C38*0.02</f>
         <v>5000</v>
       </c>
-      <c r="D42" s="83"/>
+      <c r="D42" s="66"/>
       <c r="E42" s="39">
         <v>2</v>
       </c>
@@ -2198,7 +2201,7 @@
       <c r="J42" s="48"/>
       <c r="K42" s="49"/>
     </row>
-    <row r="43" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="57"/>
       <c r="B43" s="57"/>
       <c r="C43" s="57"/>
@@ -2211,64 +2214,71 @@
       <c r="J43" s="57"/>
       <c r="K43" s="57"/>
     </row>
-    <row r="44" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="49" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="50" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="51" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="52" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="53" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="54" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="55" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="56" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="57" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="58" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="59" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="63" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="73" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="79" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="81" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="90" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="91" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="93" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="94" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="95" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="96" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="97" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="98" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="99" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="A7:F7"/>
@@ -2277,13 +2287,6 @@
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -2300,110 +2303,110 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-    </row>
-    <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="68" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+    </row>
+    <row r="2" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="69" t="s">
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="69" t="s">
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+    </row>
+    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-    </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="70" t="s">
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+    </row>
+    <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="70"/>
-      <c r="K5" s="70"/>
-    </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="87"/>
+      <c r="K5" s="87"/>
+    </row>
+    <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="65">
+      <c r="C6" s="83">
         <f>F29</f>
         <v>309587.38791333331</v>
       </c>
-      <c r="D6" s="66"/>
+      <c r="D6" s="84"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -2411,90 +2414,90 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="65">
+      <c r="J6" s="83">
         <f>I29</f>
-        <v>262421.84455559734</v>
-      </c>
-      <c r="K6" s="66"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>245590.98382323494</v>
+      </c>
+      <c r="K6" s="84"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="I7" s="75" t="s">
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="I7" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="73" t="e">
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="70" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="I8" s="76" t="s">
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="I8" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="76"/>
-      <c r="K8" s="76"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="77" t="e">
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="81" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="77"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="I9" s="76" t="s">
+      <c r="B9" s="81"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
+      <c r="I9" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="76"/>
-      <c r="K9" s="76"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="71" t="s">
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="71" t="s">
+      <c r="C11" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="78" t="s">
+      <c r="D11" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="78" t="s">
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="71" t="s">
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="72" t="s">
+      <c r="K11" s="77" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="71"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="71"/>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="76"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -2513,10 +2516,10 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="71"/>
-      <c r="K12" s="72"/>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="J12" s="76"/>
+      <c r="K12" s="77"/>
+    </row>
+    <row r="13" spans="1:13" s="1" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
         <f>'200k'!A9</f>
         <v>1</v>
@@ -2542,26 +2545,30 @@
         <v>1244.1274999999998</v>
       </c>
       <c r="G13" s="12">
-        <f>V!G11</f>
-        <v>14.761687500000001</v>
+        <f>V!G12</f>
+        <v>24.563025</v>
       </c>
       <c r="H13" s="12">
-        <f>V!I11</f>
+        <f>V!I12</f>
         <v>64.63</v>
       </c>
       <c r="I13" s="12">
         <f>G13*H13</f>
-        <v>954.04786312499994</v>
+        <v>1587.5083057499999</v>
       </c>
       <c r="J13" s="28">
         <f>I13-F13</f>
-        <v>-290.07963687499989</v>
+        <v>343.38080575000004</v>
       </c>
       <c r="K13" s="14"/>
-    </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M13" s="1">
+        <f>1.25*F13</f>
+        <v>1555.1593749999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="27"/>
-      <c r="B14" s="87" t="str">
+      <c r="B14" s="65" t="str">
         <f>'200k'!B12</f>
         <v>VAT calculation</v>
       </c>
@@ -2575,16 +2582,20 @@
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12">
-        <f>V!J12</f>
-        <v>102.79547118750001</v>
+        <f>V!J13</f>
+        <v>171.048718425</v>
       </c>
       <c r="J14" s="28">
         <f>I14-F14</f>
-        <v>-31.255112145833309</v>
+        <v>36.998135091666683</v>
       </c>
       <c r="K14" s="14"/>
-    </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M14" s="1">
+        <f>1.25*F14</f>
+        <v>167.56322916666664</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29"/>
       <c r="B15" s="29"/>
       <c r="C15" s="12"/>
@@ -2597,7 +2608,7 @@
       <c r="J15" s="28"/>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" s="1" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A16" s="27">
         <f>'200k'!A14</f>
         <v>2</v>
@@ -2623,11 +2634,11 @@
         <v>2918.3962499999998</v>
       </c>
       <c r="G16" s="12">
-        <f>V!G17</f>
+        <f>V!G18</f>
         <v>0</v>
       </c>
       <c r="H16" s="12">
-        <f>V!I17</f>
+        <f>V!I18</f>
         <v>404.28</v>
       </c>
       <c r="I16" s="12">
@@ -2639,8 +2650,12 @@
         <v>-2918.3962499999998</v>
       </c>
       <c r="K16" s="14"/>
-    </row>
-    <row r="17" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M16" s="1">
+        <f>1.25*F16</f>
+        <v>3647.9953124999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="27"/>
       <c r="B17" s="32"/>
       <c r="C17" s="12"/>
@@ -2653,7 +2668,7 @@
       <c r="J17" s="28"/>
       <c r="K17" s="14"/>
     </row>
-    <row r="18" spans="1:13" s="1" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" s="1" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A18" s="27">
         <f>'200k'!A18</f>
         <v>3</v>
@@ -2679,20 +2694,20 @@
         <v>7316.9580000000005</v>
       </c>
       <c r="G18" s="12">
-        <f>V!G26</f>
-        <v>2.5305750000000002</v>
+        <f>V!G27</f>
+        <v>2.42055</v>
       </c>
       <c r="H18" s="12">
-        <f>V!I26</f>
+        <f>V!I27</f>
         <v>4434.5200000000004</v>
       </c>
       <c r="I18" s="12">
         <f>G18*H18</f>
-        <v>11221.885449000003</v>
+        <v>10733.977386</v>
       </c>
       <c r="J18" s="28">
         <f>I18-F18</f>
-        <v>3904.9274490000025</v>
+        <v>3417.0193859999999</v>
       </c>
       <c r="K18" s="14"/>
       <c r="M18" s="1">
@@ -2700,9 +2715,9 @@
         <v>9146.1975000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="27"/>
-      <c r="B19" s="87" t="str">
+      <c r="B19" s="65" t="str">
         <f>'200k'!B21</f>
         <v>VAT calculation</v>
       </c>
@@ -2716,16 +2731,20 @@
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
       <c r="I19" s="12">
-        <f>V!J27</f>
-        <v>974.92325112000015</v>
+        <f>V!J28</f>
+        <v>932.53528368000002</v>
       </c>
       <c r="J19" s="28">
         <f>I19-F19</f>
-        <v>339.24821112000018</v>
+        <v>296.86024368000005</v>
       </c>
       <c r="K19" s="14"/>
-    </row>
-    <row r="20" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M19" s="1">
+        <f>1.25*F19</f>
+        <v>794.59379999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="27"/>
       <c r="B20" s="32"/>
       <c r="C20" s="12"/>
@@ -2738,7 +2757,7 @@
       <c r="J20" s="28"/>
       <c r="K20" s="14"/>
     </row>
-    <row r="21" spans="1:13" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A21" s="27">
         <f>'200k'!A23</f>
         <v>4</v>
@@ -2764,11 +2783,11 @@
         <v>8773.4624999999996</v>
       </c>
       <c r="G21" s="12">
-        <f>V!G31</f>
+        <f>V!G32</f>
         <v>0</v>
       </c>
       <c r="H21" s="12">
-        <f>V!I31</f>
+        <f>V!I32</f>
         <v>10634.5</v>
       </c>
       <c r="I21" s="12">
@@ -2780,10 +2799,14 @@
         <v>-8773.4624999999996</v>
       </c>
       <c r="K21" s="14"/>
-    </row>
-    <row r="22" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M21" s="1">
+        <f>1.25*F21</f>
+        <v>10966.828125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="27"/>
-      <c r="B22" s="87" t="str">
+      <c r="B22" s="65" t="str">
         <f>'200k'!B26</f>
         <v>VAT calculation</v>
       </c>
@@ -2797,7 +2820,7 @@
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12">
-        <f>V!J32</f>
+        <f>V!J33</f>
         <v>0</v>
       </c>
       <c r="J22" s="28">
@@ -2805,8 +2828,12 @@
         <v>-865.45459000000005</v>
       </c>
       <c r="K22" s="14"/>
-    </row>
-    <row r="23" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M22" s="1">
+        <f>1.25*F22</f>
+        <v>1081.8182375000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="27"/>
       <c r="B23" s="32"/>
       <c r="C23" s="12"/>
@@ -2819,7 +2846,7 @@
       <c r="J23" s="28"/>
       <c r="K23" s="14"/>
     </row>
-    <row r="24" spans="1:13" s="1" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" s="1" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A24" s="27">
         <f>'200k'!A28</f>
         <v>5</v>
@@ -2845,26 +2872,30 @@
         <v>264645.42499999999</v>
       </c>
       <c r="G24" s="12">
-        <f>V!G41</f>
-        <v>23.810560000000002</v>
+        <f>V!G42</f>
+        <v>22.182552148735144</v>
       </c>
       <c r="H24" s="12">
-        <f>V!I41</f>
+        <f>V!I42</f>
         <v>9623.4699999999993</v>
       </c>
       <c r="I24" s="12">
         <f>G24*H24</f>
-        <v>229140.20984320002</v>
+        <v>213473.12512678819</v>
       </c>
       <c r="J24" s="28">
         <f>I24-F24</f>
-        <v>-35505.215156799968</v>
+        <v>-51172.299873211799</v>
       </c>
       <c r="K24" s="14"/>
-    </row>
-    <row r="25" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M24" s="1">
+        <f>1.25*F24</f>
+        <v>330806.78125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="27"/>
-      <c r="B25" s="87" t="str">
+      <c r="B25" s="65" t="str">
         <f>'200k'!B31</f>
         <v>VAT calculation</v>
       </c>
@@ -2878,16 +2909,20 @@
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
       <c r="I25" s="12">
-        <f>V!J42</f>
-        <v>19527.982677964803</v>
+        <f>V!J43</f>
+        <v>18192.78900259174</v>
       </c>
       <c r="J25" s="28">
         <f>I25-F25</f>
-        <v>-3025.8557720352001</v>
+        <v>-4361.0494474082625</v>
       </c>
       <c r="K25" s="14"/>
-    </row>
-    <row r="26" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M25" s="1">
+        <f>1.25*F25</f>
+        <v>28192.298062500005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="27"/>
       <c r="B26" s="32"/>
       <c r="C26" s="12"/>
@@ -2900,7 +2935,7 @@
       <c r="J26" s="28"/>
       <c r="K26" s="14"/>
     </row>
-    <row r="27" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="27">
         <f>'200k'!A33</f>
         <v>6</v>
@@ -2926,11 +2961,11 @@
         <v>500</v>
       </c>
       <c r="G27" s="12">
-        <f>V!G44</f>
+        <f>V!G45</f>
         <v>1</v>
       </c>
       <c r="H27" s="12">
-        <f>V!I44</f>
+        <f>V!I45</f>
         <v>500</v>
       </c>
       <c r="I27" s="12">
@@ -2942,8 +2977,12 @@
         <v>0</v>
       </c>
       <c r="K27" s="14"/>
-    </row>
-    <row r="28" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M27" s="1">
+        <f>1.25*F27</f>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29"/>
       <c r="B28" s="29"/>
       <c r="C28" s="12"/>
@@ -2956,7 +2995,7 @@
       <c r="J28" s="28"/>
       <c r="K28" s="14"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="6" t="s">
         <v>16</v>
@@ -2972,16 +3011,23 @@
       <c r="H29" s="7"/>
       <c r="I29" s="7">
         <f>SUM(I13:I27)</f>
-        <v>262421.84455559734</v>
+        <v>245590.98382323494</v>
       </c>
       <c r="J29" s="13">
         <f>I29-F29</f>
-        <v>-47165.543357735965</v>
+        <v>-63996.404090098367</v>
       </c>
       <c r="K29" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -2995,13 +3041,6 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3017,136 +3056,136 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S110"/>
+  <dimension ref="A1:M111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.88671875" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="69" t="s">
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="69" t="s">
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-    </row>
-    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="82" t="s">
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="75" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="82"/>
-      <c r="K5" s="82"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="73" t="s">
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="79" t="s">
+      <c r="H6" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="84" t="s">
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="85" t="s">
+      <c r="H7" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="68"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -3180,11 +3219,8 @@
       <c r="K8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="N8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="124.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="63">
         <v>1</v>
       </c>
@@ -3200,14 +3236,8 @@
       <c r="I9" s="36"/>
       <c r="J9" s="36"/>
       <c r="K9" s="36"/>
-      <c r="N9" t="s">
-        <v>49</v>
-      </c>
-      <c r="O9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="37" t="s">
         <v>51</v>
@@ -3220,89 +3250,78 @@
         <v>14.67</v>
       </c>
       <c r="E10" s="38">
-        <f>E20</f>
-        <v>1.1499999999999999</v>
+        <f>E21</f>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F10" s="38">
-        <f>1.6+0.15</f>
-        <v>1.75</v>
+        <f>1.5+0.15</f>
+        <v>1.65</v>
       </c>
       <c r="G10" s="39">
         <f>PRODUCT(C10:F10)</f>
-        <v>14.761687500000001</v>
+        <v>13.313025</v>
       </c>
       <c r="H10" s="40"/>
       <c r="I10" s="40"/>
       <c r="J10" s="40"/>
       <c r="K10" s="21"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-    </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="23">
-        <f>SUM(G10:G10)</f>
-        <v>14.761687500000001</v>
-      </c>
-      <c r="H11" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="I11" s="23">
-        <v>64.63</v>
-      </c>
-      <c r="J11" s="41">
-        <f>G11*I11</f>
-        <v>954.04786312499994</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C11" s="64">
+        <v>1</v>
+      </c>
+      <c r="D11" s="38">
+        <v>15</v>
+      </c>
+      <c r="E11" s="38">
+        <v>2.5</v>
+      </c>
+      <c r="F11" s="38">
+        <v>0.3</v>
+      </c>
+      <c r="G11" s="39">
+        <f>PRODUCT(C11:F11)</f>
+        <v>11.25</v>
+      </c>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
       <c r="K11" s="21"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-    </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="37" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
       <c r="E12" s="21"/>
       <c r="F12" s="21"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="23"/>
+      <c r="G12" s="23">
+        <f>SUM(G10:G11)</f>
+        <v>24.563025</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="23">
+        <v>64.63</v>
+      </c>
       <c r="J12" s="41">
-        <f>0.13*G11*19284/360</f>
-        <v>102.79547118750001</v>
+        <f>G12*I12</f>
+        <v>1587.5083057499999</v>
       </c>
       <c r="K12" s="21"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-    </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
-      <c r="B13" s="37"/>
+      <c r="B13" s="37" t="s">
+        <v>40</v>
+      </c>
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -3310,23 +3329,15 @@
       <c r="G13" s="23"/>
       <c r="H13" s="22"/>
       <c r="I13" s="23"/>
-      <c r="J13" s="41"/>
+      <c r="J13" s="41">
+        <f>0.13*G12*19284/360</f>
+        <v>171.048718425</v>
+      </c>
       <c r="K13" s="21"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="25"/>
-    </row>
-    <row r="14" spans="1:19" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="18">
-        <v>2</v>
-      </c>
-      <c r="B14" s="30" t="s">
-        <v>52</v>
-      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
@@ -3336,129 +3347,94 @@
       <c r="I14" s="23"/>
       <c r="J14" s="41"/>
       <c r="K14" s="21"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="25"/>
-    </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="18"/>
-      <c r="B15" s="37" t="s">
+    </row>
+    <row r="15" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
+        <v>2</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="21"/>
+    </row>
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="64">
+      <c r="C16" s="64">
         <v>0</v>
       </c>
-      <c r="D15" s="38">
-        <f>D20</f>
+      <c r="D16" s="38">
+        <f>D21</f>
         <v>2.48</v>
       </c>
-      <c r="E15" s="38">
-        <f>0.75*E20</f>
-        <v>0.86249999999999993</v>
-      </c>
-      <c r="F15" s="38">
+      <c r="E16" s="38">
+        <f>0.75*E21</f>
+        <v>0.82500000000000007</v>
+      </c>
+      <c r="F16" s="38">
         <f>F10/2</f>
-        <v>0.875</v>
-      </c>
-      <c r="G15" s="39">
-        <f>PRODUCT(C15:F15)</f>
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="G16" s="39">
+        <f>PRODUCT(C16:F16)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="21"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="25"/>
-    </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="39"/>
       <c r="H16" s="40"/>
       <c r="I16" s="40"/>
       <c r="J16" s="40"/>
       <c r="K16" s="21"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="25"/>
-    </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="37"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="21"/>
+    </row>
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="23">
-        <f>SUM(G15:G15)</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="I17" s="23">
-        <v>404.28</v>
-      </c>
-      <c r="J17" s="41">
-        <f>G17*I17</f>
-        <v>0</v>
-      </c>
-      <c r="K17" s="21"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="25"/>
-      <c r="S17" s="25"/>
-    </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
-      <c r="B18" s="37"/>
       <c r="C18" s="19"/>
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
       <c r="F18" s="21"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="41"/>
+      <c r="G18" s="23">
+        <f>SUM(G16:G16)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" s="23">
+        <v>404.28</v>
+      </c>
+      <c r="J18" s="41">
+        <f>G18*I18</f>
+        <v>0</v>
+      </c>
       <c r="K18" s="21"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="25"/>
-      <c r="S18" s="25"/>
-    </row>
-    <row r="19" spans="1:19" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="18">
-        <v>3</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>43</v>
-      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="19"/>
       <c r="D19" s="20"/>
       <c r="E19" s="21"/>
@@ -3468,246 +3444,192 @@
       <c r="I19" s="23"/>
       <c r="J19" s="41"/>
       <c r="K19" s="21"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="25"/>
-      <c r="S19" s="25"/>
-    </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="37" t="str">
-        <f>B15</f>
+    </row>
+    <row r="20" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="18">
+        <v>3</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="21"/>
+    </row>
+    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="37" t="str">
+        <f>B16</f>
         <v>-Road</v>
       </c>
-      <c r="C20" s="36">
+      <c r="C21" s="36">
         <v>1</v>
       </c>
-      <c r="D20" s="38">
+      <c r="D21" s="38">
         <f>(2.48)</f>
         <v>2.48</v>
       </c>
-      <c r="E20" s="38">
-        <f>1.15</f>
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="F20" s="38">
-        <v>0.15</v>
-      </c>
-      <c r="G20" s="39">
-        <f>PRODUCT(C20:F20)</f>
-        <v>0.42779999999999996</v>
-      </c>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="21"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="25"/>
-      <c r="S20" s="25"/>
-    </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="18"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="38">
-        <v>2.48</v>
-      </c>
       <c r="E21" s="38">
-        <f t="shared" ref="E21:E25" si="0">1.15</f>
-        <v>1.1499999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F21" s="38">
         <v>0.15</v>
       </c>
       <c r="G21" s="39">
-        <f t="shared" ref="G21:G25" si="1">PRODUCT(C21:F21)</f>
-        <v>0.42779999999999996</v>
+        <f>PRODUCT(C21:F21)</f>
+        <v>0.40920000000000001</v>
       </c>
       <c r="H21" s="40"/>
       <c r="I21" s="40"/>
       <c r="J21" s="40"/>
       <c r="K21" s="21"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="25"/>
-    </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
       <c r="B22" s="37"/>
       <c r="C22" s="36"/>
       <c r="D22" s="38">
-        <v>2.42</v>
+        <v>2.48</v>
       </c>
       <c r="E22" s="38">
-        <f t="shared" si="0"/>
-        <v>1.1499999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F22" s="38">
         <v>0.15</v>
       </c>
       <c r="G22" s="39">
-        <f t="shared" si="1"/>
-        <v>0.41744999999999999</v>
+        <f t="shared" ref="G22:G26" si="0">PRODUCT(C22:F22)</f>
+        <v>0.40920000000000001</v>
       </c>
       <c r="H22" s="40"/>
       <c r="I22" s="40"/>
       <c r="J22" s="40"/>
       <c r="K22" s="21"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="25"/>
-      <c r="S22" s="25"/>
-    </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="B23" s="37"/>
       <c r="C23" s="36"/>
       <c r="D23" s="38">
-        <v>2.44</v>
+        <v>2.42</v>
       </c>
       <c r="E23" s="38">
-        <f t="shared" si="0"/>
-        <v>1.1499999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F23" s="38">
         <v>0.15</v>
       </c>
       <c r="G23" s="39">
-        <f t="shared" si="1"/>
-        <v>0.42089999999999994</v>
+        <f t="shared" si="0"/>
+        <v>0.39929999999999999</v>
       </c>
       <c r="H23" s="40"/>
       <c r="I23" s="40"/>
       <c r="J23" s="40"/>
       <c r="K23" s="21"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="25"/>
-      <c r="S23" s="25"/>
-    </row>
-    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="37"/>
       <c r="C24" s="36"/>
       <c r="D24" s="38">
-        <v>2.4500000000000002</v>
+        <v>2.44</v>
       </c>
       <c r="E24" s="38">
-        <f t="shared" si="0"/>
-        <v>1.1499999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F24" s="38">
         <v>0.15</v>
       </c>
       <c r="G24" s="39">
-        <f t="shared" si="1"/>
-        <v>0.42262499999999997</v>
+        <f t="shared" si="0"/>
+        <v>0.40260000000000001</v>
       </c>
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
       <c r="J24" s="40"/>
       <c r="K24" s="21"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="25"/>
-      <c r="S24" s="25"/>
-    </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="37"/>
       <c r="C25" s="36"/>
       <c r="D25" s="38">
-        <v>2.4</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="E25" s="38">
-        <f t="shared" si="0"/>
-        <v>1.1499999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F25" s="38">
         <v>0.15</v>
       </c>
       <c r="G25" s="39">
-        <f t="shared" si="1"/>
-        <v>0.41399999999999998</v>
+        <f t="shared" si="0"/>
+        <v>0.40425000000000005</v>
       </c>
       <c r="H25" s="40"/>
       <c r="I25" s="40"/>
       <c r="J25" s="40"/>
       <c r="K25" s="21"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="25"/>
-    </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="40"/>
-      <c r="B26" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="42"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="33">
-        <f>SUM(G20:G25)</f>
-        <v>2.5305750000000002</v>
-      </c>
-      <c r="H26" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="I26" s="33">
-        <v>4434.5200000000004</v>
-      </c>
-      <c r="J26" s="44">
-        <f>G26*I26</f>
-        <v>11221.885449000003</v>
-      </c>
-      <c r="K26" s="36"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="38">
+        <v>2.4</v>
+      </c>
+      <c r="E26" s="38">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F26" s="38">
+        <v>0.15</v>
+      </c>
+      <c r="G26" s="39">
+        <f t="shared" si="0"/>
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="21"/>
+    </row>
+    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="40"/>
       <c r="B27" s="37" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C27" s="42"/>
       <c r="D27" s="43"/>
       <c r="E27" s="43"/>
       <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="45">
-        <f>0.13*G26*(14817.6/5)</f>
-        <v>974.92325112000015</v>
+      <c r="G27" s="33">
+        <f>SUM(G21:G26)</f>
+        <v>2.42055</v>
+      </c>
+      <c r="H27" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="I27" s="33">
+        <v>4434.5200000000004</v>
+      </c>
+      <c r="J27" s="44">
+        <f>G27*I27</f>
+        <v>10733.977386</v>
       </c>
       <c r="K27" s="36"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="40"/>
-      <c r="B28" s="37"/>
+      <c r="B28" s="37" t="s">
+        <v>40</v>
+      </c>
       <c r="C28" s="42"/>
       <c r="D28" s="43"/>
       <c r="E28" s="43"/>
@@ -3715,113 +3637,99 @@
       <c r="G28" s="43"/>
       <c r="H28" s="43"/>
       <c r="I28" s="43"/>
-      <c r="J28" s="45"/>
+      <c r="J28" s="45">
+        <f>0.13*G27*(14817.6/5)</f>
+        <v>932.53528368000002</v>
+      </c>
       <c r="K28" s="36"/>
     </row>
-    <row r="29" spans="1:19" ht="69" x14ac:dyDescent="0.3">
-      <c r="A29" s="18">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="40"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="36"/>
+    </row>
+    <row r="30" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="18">
         <v>4</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B30" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="21"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="25"/>
-      <c r="S29" s="25"/>
-    </row>
-    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="18"/>
-      <c r="B30" s="37" t="str">
+      <c r="C30" s="19"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="21"/>
+    </row>
+    <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
+      <c r="B31" s="37" t="str">
         <f>B10</f>
         <v>-For wall</v>
       </c>
-      <c r="C30" s="36">
+      <c r="C31" s="36">
         <v>0</v>
       </c>
-      <c r="D30" s="38">
+      <c r="D31" s="38">
         <v>0</v>
       </c>
-      <c r="E30" s="38">
+      <c r="E31" s="38">
         <v>0</v>
       </c>
-      <c r="F30" s="38">
+      <c r="F31" s="38">
         <v>0</v>
       </c>
-      <c r="G30" s="39">
-        <f>PRODUCT(C30:F30)</f>
+      <c r="G31" s="39">
+        <f>PRODUCT(C31:F31)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
-      <c r="K30" s="21"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="25"/>
-      <c r="S30" s="25"/>
-    </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="40"/>
-      <c r="B31" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="42"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="33">
-        <f>SUM(G30:G30)</f>
-        <v>0</v>
-      </c>
-      <c r="H31" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="I31" s="33">
-        <v>10634.5</v>
-      </c>
-      <c r="J31" s="44">
-        <f>G31*I31</f>
-        <v>0</v>
-      </c>
-      <c r="K31" s="36"/>
-    </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="21"/>
+    </row>
+    <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="40"/>
       <c r="B32" s="37" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C32" s="42"/>
       <c r="D32" s="43"/>
       <c r="E32" s="43"/>
       <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="45">
-        <f>0.13*G31*((114907.3+6135.3)/15)</f>
+      <c r="G32" s="33">
+        <f>SUM(G31:G31)</f>
         <v>0</v>
       </c>
+      <c r="H32" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="I32" s="33">
+        <v>10634.5</v>
+      </c>
+      <c r="J32" s="44">
+        <f>G32*I32</f>
+        <v>0</v>
+      </c>
       <c r="K32" s="36"/>
     </row>
-    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="40"/>
-      <c r="B33" s="37"/>
+      <c r="B33" s="37" t="s">
+        <v>40</v>
+      </c>
       <c r="C33" s="42"/>
       <c r="D33" s="43"/>
       <c r="E33" s="43"/>
@@ -3829,269 +3737,224 @@
       <c r="G33" s="43"/>
       <c r="H33" s="43"/>
       <c r="I33" s="43"/>
-      <c r="J33" s="45"/>
+      <c r="J33" s="45">
+        <f>0.13*G32*((114907.3+6135.3)/15)</f>
+        <v>0</v>
+      </c>
       <c r="K33" s="36"/>
     </row>
-    <row r="34" spans="1:19" ht="110.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="18">
+    <row r="34" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="40"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="36"/>
+    </row>
+    <row r="35" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+      <c r="A35" s="18">
         <v>5</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B35" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="41"/>
-      <c r="K34" s="21"/>
-      <c r="M34" s="25"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="25"/>
-      <c r="S34" s="25"/>
-    </row>
-    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="18"/>
-      <c r="B35" s="37" t="s">
+      <c r="C35" s="19"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="41"/>
+      <c r="K35" s="21"/>
+    </row>
+    <row r="36" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="18"/>
+      <c r="B36" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="36">
+      <c r="C36" s="36">
         <v>1</v>
       </c>
-      <c r="D35" s="38">
+      <c r="D36" s="38">
         <f>(2.48)</f>
         <v>2.48</v>
       </c>
-      <c r="E35" s="38">
-        <f>((0.95+1.13)/2+(1.15))/2</f>
-        <v>1.095</v>
-      </c>
-      <c r="F35" s="38">
-        <f>1.24+0.36</f>
-        <v>1.6</v>
-      </c>
-      <c r="G35" s="39">
-        <f>PRODUCT(C35:F35)</f>
-        <v>4.3449599999999995</v>
-      </c>
-      <c r="H35" s="40"/>
-      <c r="I35" s="40"/>
-      <c r="J35" s="40"/>
-      <c r="K35" s="21"/>
-      <c r="M35" s="25"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
-      <c r="R35" s="25"/>
-      <c r="S35" s="25"/>
-    </row>
-    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="18"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="38">
-        <v>2.48</v>
-      </c>
       <c r="E36" s="38">
-        <f>((1.06+1.13)/2+(1.15))/2</f>
-        <v>1.1225000000000001</v>
+        <f>((0.95+1.13)/2+(1.1))/2</f>
+        <v>1.07</v>
       </c>
       <c r="F36" s="38">
-        <f t="shared" ref="F36:F39" si="2">1.24+0.36</f>
-        <v>1.6</v>
+        <f>5/3.281</f>
+        <v>1.5239256324291375</v>
       </c>
       <c r="G36" s="39">
-        <f t="shared" ref="G36:G40" si="3">PRODUCT(C36:F36)</f>
-        <v>4.4540800000000003</v>
+        <f>PRODUCT(C36:F36)</f>
+        <v>4.0438890582139591</v>
       </c>
       <c r="H36" s="40"/>
       <c r="I36" s="40"/>
       <c r="J36" s="40"/>
       <c r="K36" s="21"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
-      <c r="Q36" s="1"/>
-      <c r="R36" s="25"/>
-      <c r="S36" s="25"/>
-    </row>
-    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M36">
+        <f>1.04+0.52</f>
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18"/>
       <c r="B37" s="37"/>
       <c r="C37" s="36"/>
       <c r="D37" s="38">
-        <v>2.42</v>
+        <v>2.48</v>
       </c>
       <c r="E37" s="38">
-        <f>((1.06+0.95)/2+(1.15))/2</f>
-        <v>1.0774999999999999</v>
+        <f>((1.06+1.13)/2+(1.1))/2</f>
+        <v>1.0975000000000001</v>
       </c>
       <c r="F37" s="38">
-        <f t="shared" si="2"/>
-        <v>1.6</v>
+        <f t="shared" ref="F37:F40" si="1">5/3.281</f>
+        <v>1.5239256324291375</v>
       </c>
       <c r="G37" s="39">
-        <f t="shared" si="3"/>
-        <v>4.1720800000000002</v>
+        <f t="shared" ref="G37:G41" si="2">PRODUCT(C37:F37)</f>
+        <v>4.1478207863456271</v>
       </c>
       <c r="H37" s="40"/>
       <c r="I37" s="40"/>
       <c r="J37" s="40"/>
       <c r="K37" s="21"/>
-      <c r="M37" s="25"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="25"/>
-      <c r="S37" s="25"/>
-    </row>
-    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18"/>
       <c r="B38" s="37"/>
       <c r="C38" s="36"/>
       <c r="D38" s="38">
-        <v>2.44</v>
+        <v>2.42</v>
       </c>
       <c r="E38" s="38">
-        <f>((0.95+0.92)/2+(1.15))/2</f>
-        <v>1.0425</v>
+        <f>((1.06+0.95)/2+(1.1))/2</f>
+        <v>1.0525</v>
       </c>
       <c r="F38" s="38">
+        <f t="shared" si="1"/>
+        <v>1.5239256324291375</v>
+      </c>
+      <c r="G38" s="39">
         <f t="shared" si="2"/>
-        <v>1.6</v>
-      </c>
-      <c r="G38" s="39">
-        <f t="shared" si="3"/>
-        <v>4.0699199999999998</v>
+        <v>3.8815147820786349</v>
       </c>
       <c r="H38" s="40"/>
       <c r="I38" s="40"/>
       <c r="J38" s="40"/>
       <c r="K38" s="21"/>
-      <c r="M38" s="25"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="25"/>
-      <c r="S38" s="25"/>
-    </row>
-    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="18"/>
       <c r="B39" s="37"/>
       <c r="C39" s="36"/>
       <c r="D39" s="38">
-        <v>2.4500000000000002</v>
+        <v>2.44</v>
       </c>
       <c r="E39" s="38">
-        <f>((0.92+0.78)/2+(1.15))/2</f>
-        <v>1</v>
+        <f>((0.95+0.92)/2+(1.1))/2</f>
+        <v>1.0175000000000001</v>
       </c>
       <c r="F39" s="38">
+        <f t="shared" si="1"/>
+        <v>1.5239256324291375</v>
+      </c>
+      <c r="G39" s="39">
         <f t="shared" si="2"/>
-        <v>1.6</v>
-      </c>
-      <c r="G39" s="39">
-        <f t="shared" si="3"/>
-        <v>3.9200000000000004</v>
+        <v>3.7834501676318193</v>
       </c>
       <c r="H39" s="40"/>
       <c r="I39" s="40"/>
       <c r="J39" s="40"/>
       <c r="K39" s="21"/>
-      <c r="M39" s="25"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="25"/>
-      <c r="S39" s="25"/>
-    </row>
-    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18"/>
       <c r="B40" s="37"/>
       <c r="C40" s="36"/>
       <c r="D40" s="38">
-        <v>2.4</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="E40" s="38">
-        <f>((0.78+0.75)/2+(1.15))/2</f>
-        <v>0.95750000000000002</v>
+        <f>((0.92+0.78)/2+(1.1))/2</f>
+        <v>0.97500000000000009</v>
       </c>
       <c r="F40" s="38">
-        <v>1.24</v>
+        <f t="shared" si="1"/>
+        <v>1.5239256324291375</v>
       </c>
       <c r="G40" s="39">
-        <f t="shared" si="3"/>
-        <v>2.8495200000000001</v>
+        <f t="shared" si="2"/>
+        <v>3.6402773544651028</v>
       </c>
       <c r="H40" s="40"/>
       <c r="I40" s="40"/>
       <c r="J40" s="40"/>
       <c r="K40" s="21"/>
-      <c r="M40" s="25"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="25"/>
-      <c r="S40" s="25"/>
-    </row>
-    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="40"/>
-      <c r="B41" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="42"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="33">
-        <f>SUM(G35:G40)</f>
-        <v>23.810560000000002</v>
-      </c>
-      <c r="H41" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="I41" s="33">
-        <v>9623.4699999999993</v>
-      </c>
-      <c r="J41" s="44">
-        <f>G41*I41</f>
-        <v>229140.20984320002</v>
-      </c>
-      <c r="K41" s="36"/>
-    </row>
-    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="18"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="38">
+        <v>2.4</v>
+      </c>
+      <c r="E41" s="38">
+        <f>((0.78+0.75)/2+(1.1))/2</f>
+        <v>0.93250000000000011</v>
+      </c>
+      <c r="F41" s="38">
+        <v>1.2</v>
+      </c>
+      <c r="G41" s="39">
+        <f t="shared" si="2"/>
+        <v>2.6856</v>
+      </c>
+      <c r="H41" s="40"/>
+      <c r="I41" s="40"/>
+      <c r="J41" s="40"/>
+      <c r="K41" s="21"/>
+    </row>
+    <row r="42" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="40"/>
       <c r="B42" s="37" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C42" s="42"/>
       <c r="D42" s="43"/>
       <c r="E42" s="43"/>
       <c r="F42" s="43"/>
-      <c r="G42" s="43"/>
-      <c r="H42" s="43"/>
-      <c r="I42" s="43"/>
-      <c r="J42" s="45">
-        <f>0.13*G41*((59609.3+3478.36)/10)</f>
-        <v>19527.982677964803</v>
+      <c r="G42" s="33">
+        <f>SUM(G36:G41)</f>
+        <v>22.182552148735144</v>
+      </c>
+      <c r="H42" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="I42" s="33">
+        <v>9623.4699999999993</v>
+      </c>
+      <c r="J42" s="44">
+        <f>G42*I42</f>
+        <v>213473.12512678819</v>
       </c>
       <c r="K42" s="36"/>
     </row>
-    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="40"/>
-      <c r="B43" s="37"/>
+      <c r="B43" s="37" t="s">
+        <v>40</v>
+      </c>
       <c r="C43" s="42"/>
       <c r="D43" s="43"/>
       <c r="E43" s="43"/>
@@ -4099,141 +3962,128 @@
       <c r="G43" s="43"/>
       <c r="H43" s="43"/>
       <c r="I43" s="43"/>
-      <c r="J43" s="45"/>
+      <c r="J43" s="45">
+        <f>0.13*G42*((59609.3+3478.36)/10)</f>
+        <v>18192.78900259174</v>
+      </c>
       <c r="K43" s="36"/>
     </row>
-    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="18">
+    <row r="44" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="40"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="43"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="45"/>
+      <c r="K44" s="36"/>
+    </row>
+    <row r="45" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="18">
         <v>6</v>
       </c>
-      <c r="B44" s="30" t="s">
+      <c r="B45" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C44" s="19">
+      <c r="C45" s="19">
         <v>1</v>
       </c>
-      <c r="D44" s="20"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="34">
-        <f t="shared" ref="G44" si="4">PRODUCT(C44:F44)</f>
-        <v>1</v>
-      </c>
-      <c r="H44" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="I44" s="23">
-        <v>500</v>
-      </c>
-      <c r="J44" s="34">
-        <f>G44*I44</f>
-        <v>500</v>
-      </c>
-      <c r="K44" s="21"/>
-      <c r="M44" s="25"/>
-    </row>
-    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="18"/>
-      <c r="B45" s="24"/>
-      <c r="C45" s="19"/>
       <c r="D45" s="20"/>
       <c r="E45" s="21"/>
       <c r="F45" s="21"/>
-      <c r="G45" s="23"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="41"/>
+      <c r="G45" s="34">
+        <f t="shared" ref="G45" si="3">PRODUCT(C45:F45)</f>
+        <v>1</v>
+      </c>
+      <c r="H45" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I45" s="23">
+        <v>500</v>
+      </c>
+      <c r="J45" s="34">
+        <f>G45*I45</f>
+        <v>500</v>
+      </c>
       <c r="K45" s="21"/>
-      <c r="M45" s="25"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
-      <c r="P45" s="1"/>
-      <c r="Q45" s="1"/>
-      <c r="R45" s="25"/>
-      <c r="S45" s="25"/>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A46" s="40"/>
-      <c r="B46" s="46" t="s">
+    </row>
+    <row r="46" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="18"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="41"/>
+      <c r="K46" s="21"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="40"/>
+      <c r="B47" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C46" s="47"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="41"/>
-      <c r="H46" s="41"/>
-      <c r="I46" s="41"/>
-      <c r="J46" s="41">
-        <f>SUM(J10:J44)</f>
-        <v>262421.84455559734</v>
-      </c>
-      <c r="K46" s="36"/>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A47" s="58"/>
-      <c r="B47" s="61"/>
-      <c r="C47" s="62"/>
-      <c r="D47" s="59"/>
-      <c r="E47" s="59"/>
-      <c r="F47" s="59"/>
-      <c r="G47" s="60"/>
-      <c r="H47" s="60"/>
-      <c r="I47" s="60"/>
-      <c r="J47" s="60"/>
-      <c r="K47" s="57"/>
-    </row>
-    <row r="48" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="50"/>
-      <c r="B48" s="29" t="s">
+      <c r="C47" s="47"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="41"/>
+      <c r="J47" s="41">
+        <f>SUM(J10:J45)</f>
+        <v>245590.98382323494</v>
+      </c>
+      <c r="K47" s="36"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="58"/>
+      <c r="B48" s="61"/>
+      <c r="C48" s="62"/>
+      <c r="D48" s="59"/>
+      <c r="E48" s="59"/>
+      <c r="F48" s="59"/>
+      <c r="G48" s="60"/>
+      <c r="H48" s="60"/>
+      <c r="I48" s="60"/>
+      <c r="J48" s="60"/>
+      <c r="K48" s="57"/>
+    </row>
+    <row r="49" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="50"/>
+      <c r="B49" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="83">
-        <f>J46</f>
-        <v>262421.84455559734</v>
-      </c>
-      <c r="D48" s="83"/>
-      <c r="E48" s="39">
+      <c r="C49" s="66">
+        <f>J47</f>
+        <v>245590.98382323494</v>
+      </c>
+      <c r="D49" s="66"/>
+      <c r="E49" s="39">
         <v>100</v>
       </c>
-      <c r="F48" s="51"/>
-      <c r="G48" s="52"/>
-      <c r="H48" s="51"/>
-      <c r="I48" s="53"/>
-      <c r="J48" s="54"/>
-      <c r="K48" s="55"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A49" s="56"/>
-      <c r="B49" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C49" s="86">
-        <v>250000</v>
-      </c>
-      <c r="D49" s="86"/>
-      <c r="E49" s="39"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="48"/>
-      <c r="H49" s="48"/>
-      <c r="I49" s="48"/>
-      <c r="J49" s="48"/>
-      <c r="K49" s="49"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F49" s="51"/>
+      <c r="G49" s="52"/>
+      <c r="H49" s="51"/>
+      <c r="I49" s="53"/>
+      <c r="J49" s="54"/>
+      <c r="K49" s="55"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="56"/>
       <c r="B50" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C50" s="86">
-        <f>C49-C52-C53</f>
-        <v>237500</v>
-      </c>
-      <c r="D50" s="86"/>
-      <c r="E50" s="39">
-        <f>C50/C48*100</f>
-        <v>90.503136429895278</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C50" s="69">
+        <v>250000</v>
+      </c>
+      <c r="D50" s="69"/>
+      <c r="E50" s="39"/>
       <c r="F50" s="49"/>
       <c r="G50" s="48"/>
       <c r="H50" s="48"/>
@@ -4241,19 +4091,19 @@
       <c r="J50" s="48"/>
       <c r="K50" s="49"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="56"/>
       <c r="B51" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C51" s="83">
-        <f>C48-C50</f>
-        <v>24921.844555597345</v>
-      </c>
-      <c r="D51" s="83"/>
+        <v>33</v>
+      </c>
+      <c r="C51" s="69">
+        <f>C50-C53-C54</f>
+        <v>237500</v>
+      </c>
+      <c r="D51" s="69"/>
       <c r="E51" s="39">
-        <f>100-E50</f>
-        <v>9.4968635701047219</v>
+        <f>C51/C49*100</f>
+        <v>96.705504535517278</v>
       </c>
       <c r="F51" s="49"/>
       <c r="G51" s="48"/>
@@ -4262,18 +4112,19 @@
       <c r="J51" s="48"/>
       <c r="K51" s="49"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="56"/>
       <c r="B52" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C52" s="83">
-        <f>C49*0.03</f>
-        <v>7500</v>
-      </c>
-      <c r="D52" s="83"/>
+        <v>34</v>
+      </c>
+      <c r="C52" s="66">
+        <f>C49-C51</f>
+        <v>8090.983823234943</v>
+      </c>
+      <c r="D52" s="66"/>
       <c r="E52" s="39">
-        <v>3</v>
+        <f>100-E51</f>
+        <v>3.294495464482722</v>
       </c>
       <c r="F52" s="49"/>
       <c r="G52" s="48"/>
@@ -4282,18 +4133,18 @@
       <c r="J52" s="48"/>
       <c r="K52" s="49"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="56"/>
       <c r="B53" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C53" s="83">
-        <f>C49*0.02</f>
-        <v>5000</v>
-      </c>
-      <c r="D53" s="83"/>
+        <v>35</v>
+      </c>
+      <c r="C53" s="66">
+        <f>C50*0.03</f>
+        <v>7500</v>
+      </c>
+      <c r="D53" s="66"/>
       <c r="E53" s="39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F53" s="49"/>
       <c r="G53" s="48"/>
@@ -4302,92 +4153,112 @@
       <c r="J53" s="48"/>
       <c r="K53" s="49"/>
     </row>
-    <row r="54" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="57"/>
-      <c r="B54" s="57"/>
-      <c r="C54" s="57"/>
-      <c r="D54" s="57"/>
-      <c r="E54" s="57"/>
-      <c r="F54" s="57"/>
-      <c r="G54" s="57"/>
-      <c r="H54" s="57"/>
-      <c r="I54" s="57"/>
-      <c r="J54" s="57"/>
-      <c r="K54" s="57"/>
-    </row>
-    <row r="55" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="73" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="79" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="81" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="90" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="91" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="93" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="94" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="95" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="96" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="97" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="98" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="99" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="100" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="101" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="102" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="103" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="104" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="105" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="106" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="107" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="108" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="109" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="110" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="56"/>
+      <c r="B54" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" s="66">
+        <f>C50*0.02</f>
+        <v>5000</v>
+      </c>
+      <c r="D54" s="66"/>
+      <c r="E54" s="39">
+        <v>2</v>
+      </c>
+      <c r="F54" s="49"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="48"/>
+      <c r="I54" s="48"/>
+      <c r="J54" s="48"/>
+      <c r="K54" s="49"/>
+    </row>
+    <row r="55" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="57"/>
+      <c r="B55" s="57"/>
+      <c r="C55" s="57"/>
+      <c r="D55" s="57"/>
+      <c r="E55" s="57"/>
+      <c r="F55" s="57"/>
+      <c r="G55" s="57"/>
+      <c r="H55" s="57"/>
+      <c r="I55" s="57"/>
+      <c r="J55" s="57"/>
+      <c r="K55" s="57"/>
+    </row>
+    <row r="56" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>

</xml_diff>